<commit_message>
feat: 타일 맵 추가, CharacterInfo 시작 무기 수정
</commit_message>
<xml_diff>
--- a/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/CharacterInfo.xlsx
+++ b/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/CharacterInfo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\GitProject\INFEST\INFEST_Project\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42882FEB-25C9-4897-A7ED-04AA5EBF22E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279A3CD4-B4A0-429A-8431-ED3959236CCA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19245" windowHeight="8700" xr2:uid="{50378061-4796-4660-A6B7-713A0EEC2C44}"/>
   </bookViews>
@@ -546,7 +546,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -708,7 +708,7 @@
         <v>100</v>
       </c>
       <c r="J4">
-        <v>10101</v>
+        <v>10201</v>
       </c>
       <c r="K4">
         <v>10501</v>
@@ -784,7 +784,7 @@
         <v>100</v>
       </c>
       <c r="J6">
-        <v>10601</v>
+        <v>10201</v>
       </c>
       <c r="K6">
         <v>10501</v>
@@ -822,7 +822,7 @@
         <v>100</v>
       </c>
       <c r="J7">
-        <v>10401</v>
+        <v>10201</v>
       </c>
       <c r="K7">
         <v>10501</v>

</xml_diff>

<commit_message>
feat: Add Ability Data
</commit_message>
<xml_diff>
--- a/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/CharacterInfo.xlsx
+++ b/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/CharacterInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\GitProject\INFEST\INFEST_Project\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279A3CD4-B4A0-429A-8431-ED3959236CCA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CBFB41-5E84-4D0B-A5F7-3404ED12558C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19245" windowHeight="8700" xr2:uid="{50378061-4796-4660-A6B7-713A0EEC2C44}"/>
   </bookViews>
@@ -546,7 +546,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection sqref="A1:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>